<commit_message>
harmonize handling of influenza in code and data
All influenza entries in curated data now handled in unified way, no special cases, resulting in code simplification.  Several curation errors related to influenza corrected as checked data.  Vaccine lookup table updated to handle new entries.
</commit_message>
<xml_diff>
--- a/source_data/vaccine_years.xlsx
+++ b/source_data/vaccine_years.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\GitHub\hipc-dashboard-pipeline\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF17C49A-6EE3-4F53-B5B1-EA0ED6A137F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C1FAE1-FB66-4B8C-A14F-159D5350941E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="2925" windowWidth="30180" windowHeight="14475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="82">
   <si>
     <t>Year</t>
   </si>
@@ -191,9 +191,6 @@
     <t>H1N1 subtype</t>
   </si>
   <si>
-    <t>generic</t>
-  </si>
-  <si>
     <t>2005mv</t>
   </si>
   <si>
@@ -252,6 +249,24 @@
   </si>
   <si>
     <t>Influenza B virus (B/Phuket/3073/2013)</t>
+  </si>
+  <si>
+    <t>Influenza A virus</t>
+  </si>
+  <si>
+    <t>ut1</t>
+  </si>
+  <si>
+    <t>ut2</t>
+  </si>
+  <si>
+    <t>unspecified-trivalent1</t>
+  </si>
+  <si>
+    <t>unspecified-trivalent2</t>
+  </si>
+  <si>
+    <t>pan</t>
   </si>
 </sst>
 </file>
@@ -1931,13 +1946,13 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="55.5703125" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="50.42578125" customWidth="1"/>
@@ -1979,18 +1994,18 @@
         <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2">
         <v>400788</v>
@@ -2076,10 +2091,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -2090,10 +2105,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>33</v>
@@ -2102,7 +2117,7 @@
         <v>1316510</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F7">
         <v>39803</v>
@@ -2181,7 +2196,7 @@
         <v>1268360</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H10">
         <v>1089607</v>
@@ -2189,7 +2204,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -2207,7 +2222,7 @@
         <v>1268360</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H11">
         <v>1321139</v>
@@ -2233,7 +2248,7 @@
         <v>1268360</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H12">
         <v>1321139</v>
@@ -2259,7 +2274,7 @@
         <v>1321009</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H13">
         <v>1321139</v>
@@ -2267,7 +2282,7 @@
     </row>
     <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>26</v>
@@ -2285,7 +2300,7 @@
         <v>1321009</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H14">
         <v>1321139</v>
@@ -2297,7 +2312,7 @@
         <v>604436</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -2314,15 +2329,15 @@
         <v>1316510</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>26</v>
@@ -2334,10 +2349,10 @@
         <v>1316510</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I16" t="s">
         <v>52</v>
@@ -2346,7 +2361,7 @@
         <v>604436</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -2363,7 +2378,7 @@
         <v>1316510</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G17" t="s">
         <v>52</v>
@@ -2386,7 +2401,7 @@
         <v>1777792</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
         <v>52</v>
@@ -2409,7 +2424,7 @@
         <v>1777792</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19" t="s">
         <v>53</v>
@@ -2432,7 +2447,7 @@
         <v>1777792</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" t="s">
         <v>52</v>
@@ -2441,7 +2456,7 @@
         <v>604436</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -2458,7 +2473,7 @@
         <v>1777792</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" t="s">
         <v>53</v>
@@ -2467,15 +2482,15 @@
         <v>1987257</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>27</v>
+      <c r="A22" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" t="s">
         <v>33</v>
@@ -2484,29 +2499,49 @@
         <v>1316510</v>
       </c>
     </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23">
+        <v>114727</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23">
+        <v>119210</v>
+      </c>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+      <c r="H23">
+        <v>11520</v>
+      </c>
+    </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>76</v>
       </c>
       <c r="D24">
-        <v>114727</v>
+        <v>11320</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F24">
-        <v>119210</v>
-      </c>
-      <c r="G24" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24">
         <v>11520</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update vaccine years files for "Influenza B virus (B/Phuket/3073/2013)"
Add default NCBI taxonomy entry for "Influenza B virus (B/Phuket/3073/2013)" of 11520, "Influenza B virus", as it does not have its own NCBI taxonomy code.
</commit_message>
<xml_diff>
--- a/source_data/vaccine_years.xlsx
+++ b/source_data/vaccine_years.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth\Documents\GitHub\hipc-dashboard-pipeline\source_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmith\Documents\GitHub\hipc-dashboard-pipeline\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C1FAE1-FB66-4B8C-A14F-159D5350941E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="25605" windowHeight="14475" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -272,7 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -312,7 +311,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +330,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -346,7 +351,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -369,6 +374,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -650,7 +657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -659,7 +666,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" customWidth="1"/>
     <col min="4" max="4" width="35.140625" customWidth="1"/>
@@ -1942,18 +1949,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="55.5703125" customWidth="1"/>
+    <col min="3" max="3" width="55.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="50.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.140625" customWidth="1"/>
@@ -2331,9 +2338,16 @@
       <c r="E15" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="F15" s="14">
+        <v>119210</v>
+      </c>
       <c r="G15" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="H15" s="14">
+        <v>11520</v>
+      </c>
+      <c r="I15" s="15"/>
     </row>
     <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -2351,9 +2365,15 @@
       <c r="E16" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="F16" s="14">
+        <v>119210</v>
+      </c>
       <c r="G16" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="H16" s="14">
+        <v>11520</v>
+      </c>
       <c r="I16" t="s">
         <v>52</v>
       </c>
@@ -2364,7 +2384,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>2016</v>
       </c>
@@ -2387,7 +2407,7 @@
         <v>604436</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>2017</v>
       </c>
@@ -2410,7 +2430,7 @@
         <v>604436</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>2018</v>
       </c>
@@ -2433,7 +2453,7 @@
         <v>1987257</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>2017</v>
       </c>
@@ -2458,8 +2478,11 @@
       <c r="I20" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="14">
+        <v>11520</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>2018</v>
       </c>
@@ -2484,8 +2507,11 @@
       <c r="I21" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="14">
+        <v>11520</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>81</v>
       </c>
@@ -2499,7 +2525,7 @@
         <v>1316510</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
         <v>77</v>
       </c>
@@ -2515,7 +2541,7 @@
       <c r="E23" t="s">
         <v>49</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="14">
         <v>119210</v>
       </c>
       <c r="G23" t="s">
@@ -2525,7 +2551,7 @@
         <v>11520</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
         <v>78</v>
       </c>
@@ -2541,14 +2567,14 @@
       <c r="E24" t="s">
         <v>54</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="14">
         <v>11520</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K14" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="K16" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="K14" r:id="rId1"/>
+    <hyperlink ref="K16" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>

</xml_diff>